<commit_message>
termine lo de los exel(el guardado)
</commit_message>
<xml_diff>
--- a/src/principalProgram/docx/docxxx2.xlsx
+++ b/src/principalProgram/docx/docxxx2.xlsx
@@ -3059,11 +3059,11 @@
         <v>155</v>
       </c>
       <c r="G14" s="83" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H14" s="196" t="inlineStr">
         <is>
-          <t>26/02/2025</t>
+          <t>01/03/2025</t>
         </is>
       </c>
       <c r="I14" s="168" t="n"/>
@@ -16737,9 +16737,9 @@
     <mergeCell ref="C234:D234"/>
     <mergeCell ref="C211:D211"/>
     <mergeCell ref="E241:F241"/>
-    <mergeCell ref="B29:D29"/>
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B123:D123"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="H57:K57"/>
     <mergeCell ref="H38:K38"/>
     <mergeCell ref="C232:D232"/>

</xml_diff>